<commit_message>
segundo ponto feiito, so falta compact do terceiro
</commit_message>
<xml_diff>
--- a/ACUC.xlsx
+++ b/ACUC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\ambiente de trabalho\VVS\VVS_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\VVS\VVS_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AADB62-98DA-4BB8-835D-9054F5B46931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B673EB-EFBA-438B-8B6E-1160DDA8D84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="26760" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t>Nodes&amp;Edges:I</t>
   </si>
@@ -186,9 +186,6 @@
     <t>i</t>
   </si>
   <si>
-    <t>{this, data, elem}</t>
-  </si>
-  <si>
     <t>{empty, nChildren}</t>
   </si>
   <si>
@@ -262,6 +259,57 @@
   </si>
   <si>
     <t>{elem}</t>
+  </si>
+  <si>
+    <t>{i}</t>
+  </si>
+  <si>
+    <t>{i,nChildren}</t>
+  </si>
+  <si>
+    <t>{i, children, empty}</t>
+  </si>
+  <si>
+    <t>{j}</t>
+  </si>
+  <si>
+    <t>{j,nChildren}</t>
+  </si>
+  <si>
+    <t>{children,j}</t>
+  </si>
+  <si>
+    <t>{children,nChildren}</t>
+  </si>
+  <si>
+    <t>{i,capacity}</t>
+  </si>
+  <si>
+    <t>{index}</t>
+  </si>
+  <si>
+    <t>{children,i,elem}</t>
+  </si>
+  <si>
+    <t>{index,i,children,elem}</t>
+  </si>
+  <si>
+    <t>{children,elem}</t>
+  </si>
+  <si>
+    <t>(G,D)</t>
+  </si>
+  <si>
+    <t>(E,D)</t>
+  </si>
+  <si>
+    <t>isEmpty</t>
+  </si>
+  <si>
+    <t>{empty, data, elem}</t>
+  </si>
+  <si>
+    <t>{i, nChildren,empty, children}</t>
   </si>
 </sst>
 </file>
@@ -583,26 +631,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="13" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -613,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -642,29 +693,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -673,7 +730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -684,26 +741,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
@@ -712,46 +775,61 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>27</v>
@@ -759,181 +837,273 @@
       <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
-        <v>61</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" t="s">
+        <v>86</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>